<commit_message>
update nhập hàng + gửi hàng anh Tưởng
</commit_message>
<xml_diff>
--- a/TDStore/ATuongBN.xlsx
+++ b/TDStore/ATuongBN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10.NewPC\01.TDStore\04.Private\TDStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4486B79-5DD6-4386-8BDE-45EC39BF9AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E2EF02-235D-4888-B133-D71A253539B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Tên</t>
   </si>
@@ -85,13 +85,31 @@
     <t>Lãi</t>
   </si>
   <si>
-    <t>Gốc + Lãi</t>
-  </si>
-  <si>
     <t>Dell N7306 i5/8/256</t>
   </si>
   <si>
     <t>Ngày 27.2.24</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Đã ck 3.5.24</t>
+  </si>
+  <si>
+    <t>Tiền đã nhận</t>
+  </si>
+  <si>
+    <t>Dell latitude 5531 i5/16/512</t>
+  </si>
+  <si>
+    <t>X1 carbon gen 4 i5/8/128</t>
+  </si>
+  <si>
+    <t>Đã ck 28.2.24</t>
+  </si>
+  <si>
+    <t>7490C i5/8/256 HD</t>
   </si>
 </sst>
 </file>
@@ -107,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +174,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -249,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -291,13 +315,19 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +853,10 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="28"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="19"/>
       <c r="D21" s="16"/>
       <c r="E21" s="17">
@@ -847,10 +877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C647C37-EA04-418B-A0F3-D633739DA77F}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +888,7 @@
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
     <col min="2" max="3" width="14.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -876,10 +906,10 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,7 +923,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2">
         <v>5000000</v>
@@ -901,13 +931,20 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="31">
         <v>3000000</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
+        <v>3600000</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -919,34 +956,42 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="31">
         <v>6500000</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="33" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>13500000</v>
+      </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="2">
-        <f>SUM(B2:B6)</f>
-        <v>25500000</v>
-      </c>
-      <c r="C8" s="2">
-        <f>SUM(C2:C2)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
-        <f>SUM(E2:E2)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>3</v>
+      <c r="A8" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="31">
+        <v>3000000</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="31">
+        <v>3500000</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -954,42 +999,50 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>3</v>
-      </c>
+      <c r="A10" s="7"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="2">
+        <f>SUM(B2:B8)</f>
+        <v>42000000</v>
+      </c>
+      <c r="C11" s="2">
+        <f>SUM(C2:C2)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <f>SUM(E2:E2)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>3</v>
+      </c>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="E14" s="14">
-        <f>SUM(E11:E13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>3</v>
-      </c>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -999,22 +1052,40 @@
       <c r="A16" s="7"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="E17" s="14">
+        <f>SUM(E14:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17">
-        <f>E8-E14</f>
+      <c r="B20" s="29"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17">
+        <f>E11-E17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F20" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>